<commit_message>
Mapeamento Conferência LN - NFV
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_NFV.xlsx
+++ b/Documentação/Planilhas/Conferencia_NFV.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="558">
   <si>
     <t>1</t>
   </si>
@@ -1552,6 +1552,165 @@
   </si>
   <si>
     <t>stg_nfv_eletronica</t>
+  </si>
+  <si>
+    <t>NF_NFE</t>
+  </si>
+  <si>
+    <t>NR_SERIE_NFE</t>
+  </si>
+  <si>
+    <t>NR_PROTOCOLO</t>
+  </si>
+  <si>
+    <t>NR_CHAVE_ACESSO_NFE</t>
+  </si>
+  <si>
+    <t>DT_STATUS</t>
+  </si>
+  <si>
+    <t>DT_CANCELAMENTO</t>
+  </si>
+  <si>
+    <t>CD_MOTIVO_CANCELAMENTO</t>
+  </si>
+  <si>
+    <t>25483</t>
+  </si>
+  <si>
+    <t>2014-06-04 16:36:02.000</t>
+  </si>
+  <si>
+    <t>F30000146</t>
+  </si>
+  <si>
+    <t>2014-09-05 11:42:29.000</t>
+  </si>
+  <si>
+    <t>33131009358108001016550020000000271797842446</t>
+  </si>
+  <si>
+    <t>2013-10-04 10:17:44.000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>135140003834255</t>
+  </si>
+  <si>
+    <t>35140709358108000206550040000001621311139490</t>
+  </si>
+  <si>
+    <t>2014-07-31 10:35:29.000</t>
+  </si>
+  <si>
+    <t>F20000224</t>
+  </si>
+  <si>
+    <t>2014-07-31 10:35:33.000</t>
+  </si>
+  <si>
+    <t>F20000337</t>
+  </si>
+  <si>
+    <t>2014-08-18 16:15:25.000</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>135140004093084</t>
+  </si>
+  <si>
+    <t>35140809358108000206550040000001691540433994</t>
+  </si>
+  <si>
+    <t>2014-08-13 17:55:32.000</t>
+  </si>
+  <si>
+    <t>F20000382</t>
+  </si>
+  <si>
+    <t>2014-08-13 17:56:03.000</t>
+  </si>
+  <si>
+    <t>2014-03-19 16:49:47.000</t>
+  </si>
+  <si>
+    <t>100000018</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>F20000435</t>
+  </si>
+  <si>
+    <t>2014-09-03 15:55:05.000</t>
+  </si>
+  <si>
+    <t>1523</t>
+  </si>
+  <si>
+    <t>2014-09-03 16:02:12.000</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>F20000493</t>
+  </si>
+  <si>
+    <t>2014-09-03 16:17:03.000</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>F20000574</t>
+  </si>
+  <si>
+    <t>2014-09-05 11:37:45.000</t>
+  </si>
+  <si>
+    <t>25480</t>
+  </si>
+  <si>
+    <t>2014-06-04 11:34:10.000</t>
+  </si>
+  <si>
+    <t>F30000143</t>
+  </si>
+  <si>
+    <t>2014-09-05 11:42:27.000</t>
+  </si>
+  <si>
+    <t>Sessão cislil504m00l (Nota Fiscal)</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ref fiscal. Na aba superior "NF-e", seção "NF-e", pegar a informação de "Protocolo NF-e"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ref fiscal. Na aba superior "NF-e", seção "NF-e", pegar a informação de "Localizador"</t>
+  </si>
+  <si>
+    <t>brnfel520m00l (Histórico de transmissão da Nfe)</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ref fiscal. Na aba superior "NF-e", seção "NF-e", pegar a informação de "Código da razão do cancelamento"</t>
+  </si>
+  <si>
+    <t>Informar a Ref Fiscal na lupinha, limpando primeiramente todos os campos. Em seguinda, pegar a informação do campo "Data". A data mais antiga para o status da transmissão como "Cancelada"</t>
+  </si>
+  <si>
+    <t>cislil504m00l, brnfel520m00l, tcmcs0565m000 e tcemm0130m000</t>
+  </si>
+  <si>
+    <t>Informar a Ref Fiscal na lupinha, limpando primeiramente todos os campos. Em seguinda, pegar a informação do campo "Data". A data mais antiga para o mesmo status da transmissão existente na Nota fiscal. Caso não tenha o mesmo status, pegar a maior data existente</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1833,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1747,11 +1906,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1820,11 +1997,38 @@
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1835,38 +2039,14 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1877,8 +2057,17 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2189,9 +2378,7 @@
   </sheetPr>
   <dimension ref="A1:AV135"/>
   <sheetViews>
-    <sheetView topLeftCell="AR4" workbookViewId="0">
-      <selection activeCell="AR17" sqref="AR17:AS26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -2247,10 +2434,10 @@
       <c r="AU1" s="4"/>
     </row>
     <row r="2" spans="1:48" ht="21">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="5" t="s">
         <v>57</v>
       </c>
@@ -2258,10 +2445,10 @@
       <c r="AU2" s="4"/>
     </row>
     <row r="3" spans="1:48" ht="21">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="5" t="s">
         <v>304</v>
       </c>
@@ -3867,626 +4054,626 @@
       <c r="AV16" s="3"/>
     </row>
     <row r="17" spans="1:48">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="24"/>
-      <c r="AD17" s="24"/>
-      <c r="AE17" s="24"/>
-      <c r="AF17" s="24"/>
-      <c r="AG17" s="24"/>
-      <c r="AH17" s="24"/>
-      <c r="AI17" s="24"/>
-      <c r="AJ17" s="24"/>
-      <c r="AK17" s="24"/>
-      <c r="AL17" s="24"/>
-      <c r="AM17" s="24"/>
-      <c r="AN17" s="24" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="32"/>
+      <c r="AB17" s="32"/>
+      <c r="AC17" s="32"/>
+      <c r="AD17" s="32"/>
+      <c r="AE17" s="32"/>
+      <c r="AF17" s="32"/>
+      <c r="AG17" s="32"/>
+      <c r="AH17" s="32"/>
+      <c r="AI17" s="32"/>
+      <c r="AJ17" s="32"/>
+      <c r="AK17" s="32"/>
+      <c r="AL17" s="32"/>
+      <c r="AM17" s="32"/>
+      <c r="AN17" s="32" t="s">
         <v>302</v>
       </c>
-      <c r="AO17" s="24"/>
-      <c r="AP17" s="24"/>
-      <c r="AQ17" s="25" t="s">
+      <c r="AO17" s="32"/>
+      <c r="AP17" s="32"/>
+      <c r="AQ17" s="40" t="s">
         <v>303</v>
       </c>
-      <c r="AR17" s="25" t="s">
+      <c r="AR17" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="AS17" s="25" t="s">
+      <c r="AS17" s="40" t="s">
         <v>295</v>
       </c>
-      <c r="AT17" s="25" t="s">
+      <c r="AT17" s="40" t="s">
         <v>291</v>
       </c>
       <c r="AU17" s="1"/>
       <c r="AV17" s="3"/>
     </row>
     <row r="18" spans="1:48">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="24"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
-      <c r="AD18" s="24"/>
-      <c r="AE18" s="24"/>
-      <c r="AF18" s="24"/>
-      <c r="AG18" s="24"/>
-      <c r="AH18" s="24"/>
-      <c r="AI18" s="24"/>
-      <c r="AJ18" s="24"/>
-      <c r="AK18" s="24"/>
-      <c r="AL18" s="24"/>
-      <c r="AM18" s="24"/>
-      <c r="AN18" s="24"/>
-      <c r="AO18" s="24"/>
-      <c r="AP18" s="24"/>
-      <c r="AQ18" s="25"/>
-      <c r="AR18" s="25"/>
-      <c r="AS18" s="25"/>
-      <c r="AT18" s="25"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="32"/>
+      <c r="AA18" s="32"/>
+      <c r="AB18" s="32"/>
+      <c r="AC18" s="32"/>
+      <c r="AD18" s="32"/>
+      <c r="AE18" s="32"/>
+      <c r="AF18" s="32"/>
+      <c r="AG18" s="32"/>
+      <c r="AH18" s="32"/>
+      <c r="AI18" s="32"/>
+      <c r="AJ18" s="32"/>
+      <c r="AK18" s="32"/>
+      <c r="AL18" s="32"/>
+      <c r="AM18" s="32"/>
+      <c r="AN18" s="32"/>
+      <c r="AO18" s="32"/>
+      <c r="AP18" s="32"/>
+      <c r="AQ18" s="40"/>
+      <c r="AR18" s="40"/>
+      <c r="AS18" s="40"/>
+      <c r="AT18" s="40"/>
       <c r="AU18" s="1"/>
       <c r="AV18" s="3"/>
     </row>
     <row r="19" spans="1:48">
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
-      <c r="AD19" s="24"/>
-      <c r="AE19" s="24"/>
-      <c r="AF19" s="24"/>
-      <c r="AG19" s="24"/>
-      <c r="AH19" s="24"/>
-      <c r="AI19" s="24"/>
-      <c r="AJ19" s="24"/>
-      <c r="AK19" s="24"/>
-      <c r="AL19" s="24"/>
-      <c r="AM19" s="24"/>
-      <c r="AN19" s="24"/>
-      <c r="AO19" s="24"/>
-      <c r="AP19" s="24"/>
-      <c r="AQ19" s="25"/>
-      <c r="AR19" s="25"/>
-      <c r="AS19" s="25"/>
-      <c r="AT19" s="25"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="32"/>
+      <c r="AB19" s="32"/>
+      <c r="AC19" s="32"/>
+      <c r="AD19" s="32"/>
+      <c r="AE19" s="32"/>
+      <c r="AF19" s="32"/>
+      <c r="AG19" s="32"/>
+      <c r="AH19" s="32"/>
+      <c r="AI19" s="32"/>
+      <c r="AJ19" s="32"/>
+      <c r="AK19" s="32"/>
+      <c r="AL19" s="32"/>
+      <c r="AM19" s="32"/>
+      <c r="AN19" s="32"/>
+      <c r="AO19" s="32"/>
+      <c r="AP19" s="32"/>
+      <c r="AQ19" s="40"/>
+      <c r="AR19" s="40"/>
+      <c r="AS19" s="40"/>
+      <c r="AT19" s="40"/>
       <c r="AU19" s="1"/>
       <c r="AV19" s="3"/>
     </row>
     <row r="20" spans="1:48" ht="11.25" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="29" t="s">
         <v>290</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="J20" s="33" t="s">
+      <c r="J20" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="M20" s="34" t="s">
+      <c r="M20" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="N20" s="34" t="s">
+      <c r="N20" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="P20" s="34" t="s">
+      <c r="P20" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="Q20" s="34" t="s">
+      <c r="Q20" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="R20" s="34" t="s">
+      <c r="R20" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="S20" s="34" t="s">
+      <c r="S20" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="T20" s="34" t="s">
+      <c r="T20" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="U20" s="34" t="s">
+      <c r="U20" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="V20" s="39" t="s">
+      <c r="V20" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="W20" s="34" t="s">
+      <c r="W20" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="X20" s="34" t="s">
+      <c r="X20" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="Y20" s="39" t="s">
+      <c r="Y20" s="27" t="s">
         <v>275</v>
       </c>
-      <c r="Z20" s="34" t="s">
+      <c r="Z20" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="AA20" s="34" t="s">
+      <c r="AA20" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="AB20" s="34" t="s">
+      <c r="AB20" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="AC20" s="34" t="s">
+      <c r="AC20" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="AD20" s="34" t="s">
+      <c r="AD20" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="AE20" s="34" t="s">
+      <c r="AE20" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="AF20" s="34" t="s">
+      <c r="AF20" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="AG20" s="39" t="s">
+      <c r="AG20" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="AH20" s="34" t="s">
+      <c r="AH20" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="AI20" s="39" t="s">
+      <c r="AI20" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="AJ20" s="36" t="s">
+      <c r="AJ20" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="AK20" s="34" t="s">
+      <c r="AK20" s="26" t="s">
         <v>279</v>
       </c>
-      <c r="AL20" s="34" t="s">
+      <c r="AL20" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="AM20" s="34" t="s">
+      <c r="AM20" s="26" t="s">
         <v>276</v>
       </c>
-      <c r="AN20" s="29" t="s">
+      <c r="AN20" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="AO20" s="29" t="s">
+      <c r="AO20" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="AP20" s="29" t="s">
+      <c r="AP20" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="AQ20" s="31" t="s">
+      <c r="AQ20" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="AR20" s="27" t="s">
+      <c r="AR20" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="AS20" s="28" t="s">
+      <c r="AS20" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="AT20" s="26" t="s">
+      <c r="AT20" s="35" t="s">
         <v>292</v>
       </c>
-      <c r="AU20" s="30" t="s">
+      <c r="AU20" s="38" t="s">
         <v>300</v>
       </c>
       <c r="AV20" s="3"/>
     </row>
     <row r="21" spans="1:48">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="34"/>
-      <c r="U21" s="34"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="39"/>
-      <c r="Z21" s="34"/>
-      <c r="AA21" s="34"/>
-      <c r="AB21" s="34"/>
-      <c r="AC21" s="34"/>
-      <c r="AD21" s="34"/>
-      <c r="AE21" s="34"/>
-      <c r="AF21" s="34"/>
-      <c r="AG21" s="39"/>
-      <c r="AH21" s="34"/>
-      <c r="AI21" s="39"/>
-      <c r="AJ21" s="36"/>
-      <c r="AK21" s="34"/>
-      <c r="AL21" s="34"/>
-      <c r="AM21" s="34"/>
-      <c r="AN21" s="29"/>
-      <c r="AO21" s="29"/>
-      <c r="AP21" s="29"/>
-      <c r="AQ21" s="31"/>
-      <c r="AR21" s="27"/>
-      <c r="AS21" s="28"/>
-      <c r="AT21" s="26"/>
-      <c r="AU21" s="30"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
+      <c r="AC21" s="26"/>
+      <c r="AD21" s="26"/>
+      <c r="AE21" s="26"/>
+      <c r="AF21" s="26"/>
+      <c r="AG21" s="27"/>
+      <c r="AH21" s="26"/>
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="28"/>
+      <c r="AK21" s="26"/>
+      <c r="AL21" s="26"/>
+      <c r="AM21" s="26"/>
+      <c r="AN21" s="25"/>
+      <c r="AO21" s="25"/>
+      <c r="AP21" s="25"/>
+      <c r="AQ21" s="39"/>
+      <c r="AR21" s="36"/>
+      <c r="AS21" s="37"/>
+      <c r="AT21" s="35"/>
+      <c r="AU21" s="38"/>
       <c r="AV21" s="3"/>
     </row>
     <row r="22" spans="1:48">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="34"/>
-      <c r="Q22" s="34"/>
-      <c r="R22" s="34"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="34"/>
-      <c r="U22" s="34"/>
-      <c r="V22" s="39"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="39"/>
-      <c r="Z22" s="34"/>
-      <c r="AA22" s="34"/>
-      <c r="AB22" s="34"/>
-      <c r="AC22" s="34"/>
-      <c r="AD22" s="34"/>
-      <c r="AE22" s="34"/>
-      <c r="AF22" s="34"/>
-      <c r="AG22" s="39"/>
-      <c r="AH22" s="34"/>
-      <c r="AI22" s="39"/>
-      <c r="AJ22" s="36"/>
-      <c r="AK22" s="34"/>
-      <c r="AL22" s="34"/>
-      <c r="AM22" s="34"/>
-      <c r="AN22" s="29"/>
-      <c r="AO22" s="29"/>
-      <c r="AP22" s="29"/>
-      <c r="AQ22" s="31"/>
-      <c r="AR22" s="27"/>
-      <c r="AS22" s="28"/>
-      <c r="AT22" s="26"/>
-      <c r="AU22" s="30"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="26"/>
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="26"/>
+      <c r="AF22" s="26"/>
+      <c r="AG22" s="27"/>
+      <c r="AH22" s="26"/>
+      <c r="AI22" s="27"/>
+      <c r="AJ22" s="28"/>
+      <c r="AK22" s="26"/>
+      <c r="AL22" s="26"/>
+      <c r="AM22" s="26"/>
+      <c r="AN22" s="25"/>
+      <c r="AO22" s="25"/>
+      <c r="AP22" s="25"/>
+      <c r="AQ22" s="39"/>
+      <c r="AR22" s="36"/>
+      <c r="AS22" s="37"/>
+      <c r="AT22" s="35"/>
+      <c r="AU22" s="38"/>
       <c r="AV22" s="3"/>
     </row>
     <row r="23" spans="1:48">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="34"/>
-      <c r="Q23" s="34"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="34"/>
-      <c r="U23" s="34"/>
-      <c r="V23" s="39"/>
-      <c r="W23" s="34"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="39"/>
-      <c r="Z23" s="34"/>
-      <c r="AA23" s="34"/>
-      <c r="AB23" s="34"/>
-      <c r="AC23" s="34"/>
-      <c r="AD23" s="34"/>
-      <c r="AE23" s="34"/>
-      <c r="AF23" s="34"/>
-      <c r="AG23" s="39"/>
-      <c r="AH23" s="34"/>
-      <c r="AI23" s="39"/>
-      <c r="AJ23" s="36"/>
-      <c r="AK23" s="34"/>
-      <c r="AL23" s="34"/>
-      <c r="AM23" s="34"/>
-      <c r="AN23" s="29"/>
-      <c r="AO23" s="29"/>
-      <c r="AP23" s="29"/>
-      <c r="AQ23" s="31"/>
-      <c r="AR23" s="27"/>
-      <c r="AS23" s="28"/>
-      <c r="AT23" s="26"/>
-      <c r="AU23" s="30"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="26"/>
+      <c r="T23" s="26"/>
+      <c r="U23" s="26"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="26"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="26"/>
+      <c r="AD23" s="26"/>
+      <c r="AE23" s="26"/>
+      <c r="AF23" s="26"/>
+      <c r="AG23" s="27"/>
+      <c r="AH23" s="26"/>
+      <c r="AI23" s="27"/>
+      <c r="AJ23" s="28"/>
+      <c r="AK23" s="26"/>
+      <c r="AL23" s="26"/>
+      <c r="AM23" s="26"/>
+      <c r="AN23" s="25"/>
+      <c r="AO23" s="25"/>
+      <c r="AP23" s="25"/>
+      <c r="AQ23" s="39"/>
+      <c r="AR23" s="36"/>
+      <c r="AS23" s="37"/>
+      <c r="AT23" s="35"/>
+      <c r="AU23" s="38"/>
       <c r="AV23" s="3"/>
     </row>
     <row r="24" spans="1:48">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="34"/>
-      <c r="V24" s="39"/>
-      <c r="W24" s="34"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="39"/>
-      <c r="Z24" s="34"/>
-      <c r="AA24" s="34"/>
-      <c r="AB24" s="34"/>
-      <c r="AC24" s="34"/>
-      <c r="AD24" s="34"/>
-      <c r="AE24" s="34"/>
-      <c r="AF24" s="34"/>
-      <c r="AG24" s="39"/>
-      <c r="AH24" s="34"/>
-      <c r="AI24" s="39"/>
-      <c r="AJ24" s="36"/>
-      <c r="AK24" s="34"/>
-      <c r="AL24" s="34"/>
-      <c r="AM24" s="34"/>
-      <c r="AN24" s="29"/>
-      <c r="AO24" s="29"/>
-      <c r="AP24" s="29"/>
-      <c r="AQ24" s="31"/>
-      <c r="AR24" s="27"/>
-      <c r="AS24" s="28"/>
-      <c r="AT24" s="26"/>
-      <c r="AU24" s="30"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="26"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="26"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="26"/>
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="26"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="27"/>
+      <c r="AH24" s="26"/>
+      <c r="AI24" s="27"/>
+      <c r="AJ24" s="28"/>
+      <c r="AK24" s="26"/>
+      <c r="AL24" s="26"/>
+      <c r="AM24" s="26"/>
+      <c r="AN24" s="25"/>
+      <c r="AO24" s="25"/>
+      <c r="AP24" s="25"/>
+      <c r="AQ24" s="39"/>
+      <c r="AR24" s="36"/>
+      <c r="AS24" s="37"/>
+      <c r="AT24" s="35"/>
+      <c r="AU24" s="38"/>
       <c r="AV24" s="3"/>
     </row>
     <row r="25" spans="1:48">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
-      <c r="V25" s="39"/>
-      <c r="W25" s="34"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="39"/>
-      <c r="Z25" s="34"/>
-      <c r="AA25" s="34"/>
-      <c r="AB25" s="34"/>
-      <c r="AC25" s="34"/>
-      <c r="AD25" s="34"/>
-      <c r="AE25" s="34"/>
-      <c r="AF25" s="34"/>
-      <c r="AG25" s="39"/>
-      <c r="AH25" s="34"/>
-      <c r="AI25" s="39"/>
-      <c r="AJ25" s="36"/>
-      <c r="AK25" s="34"/>
-      <c r="AL25" s="34"/>
-      <c r="AM25" s="34"/>
-      <c r="AN25" s="29"/>
-      <c r="AO25" s="29"/>
-      <c r="AP25" s="29"/>
-      <c r="AQ25" s="31"/>
-      <c r="AR25" s="27"/>
-      <c r="AS25" s="28"/>
-      <c r="AT25" s="26"/>
-      <c r="AU25" s="30"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="26"/>
+      <c r="T25" s="26"/>
+      <c r="U25" s="26"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="26"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="26"/>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="26"/>
+      <c r="AD25" s="26"/>
+      <c r="AE25" s="26"/>
+      <c r="AF25" s="26"/>
+      <c r="AG25" s="27"/>
+      <c r="AH25" s="26"/>
+      <c r="AI25" s="27"/>
+      <c r="AJ25" s="28"/>
+      <c r="AK25" s="26"/>
+      <c r="AL25" s="26"/>
+      <c r="AM25" s="26"/>
+      <c r="AN25" s="25"/>
+      <c r="AO25" s="25"/>
+      <c r="AP25" s="25"/>
+      <c r="AQ25" s="39"/>
+      <c r="AR25" s="36"/>
+      <c r="AS25" s="37"/>
+      <c r="AT25" s="35"/>
+      <c r="AU25" s="38"/>
       <c r="AV25" s="3"/>
     </row>
     <row r="26" spans="1:48">
-      <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
-      <c r="U26" s="34"/>
-      <c r="V26" s="39"/>
-      <c r="W26" s="34"/>
-      <c r="X26" s="34"/>
-      <c r="Y26" s="39"/>
-      <c r="Z26" s="34"/>
-      <c r="AA26" s="34"/>
-      <c r="AB26" s="34"/>
-      <c r="AC26" s="34"/>
-      <c r="AD26" s="34"/>
-      <c r="AE26" s="34"/>
-      <c r="AF26" s="34"/>
-      <c r="AG26" s="39"/>
-      <c r="AH26" s="34"/>
-      <c r="AI26" s="39"/>
-      <c r="AJ26" s="36"/>
-      <c r="AK26" s="34"/>
-      <c r="AL26" s="34"/>
-      <c r="AM26" s="34"/>
-      <c r="AN26" s="29"/>
-      <c r="AO26" s="29"/>
-      <c r="AP26" s="29"/>
-      <c r="AQ26" s="31"/>
-      <c r="AR26" s="27"/>
-      <c r="AS26" s="28"/>
-      <c r="AT26" s="26"/>
-      <c r="AU26" s="30"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="26"/>
+      <c r="AC26" s="26"/>
+      <c r="AD26" s="26"/>
+      <c r="AE26" s="26"/>
+      <c r="AF26" s="26"/>
+      <c r="AG26" s="27"/>
+      <c r="AH26" s="26"/>
+      <c r="AI26" s="27"/>
+      <c r="AJ26" s="28"/>
+      <c r="AK26" s="26"/>
+      <c r="AL26" s="26"/>
+      <c r="AM26" s="26"/>
+      <c r="AN26" s="25"/>
+      <c r="AO26" s="25"/>
+      <c r="AP26" s="25"/>
+      <c r="AQ26" s="39"/>
+      <c r="AR26" s="36"/>
+      <c r="AS26" s="37"/>
+      <c r="AT26" s="35"/>
+      <c r="AU26" s="38"/>
       <c r="AV26" s="3"/>
     </row>
     <row r="27" spans="1:48">
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="36" t="s">
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="28" t="s">
         <v>283</v>
       </c>
       <c r="N27" s="4"/>
       <c r="O27" s="1"/>
       <c r="T27" s="4"/>
       <c r="U27" s="1"/>
-      <c r="W27" s="34"/>
-      <c r="Z27" s="34"/>
+      <c r="W27" s="26"/>
+      <c r="Z27" s="26"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="1"/>
-      <c r="AH27" s="34"/>
-      <c r="AJ27" s="36"/>
+      <c r="AH27" s="26"/>
+      <c r="AJ27" s="28"/>
       <c r="AP27" s="4"/>
       <c r="AQ27" s="1"/>
       <c r="AU27" s="1"/>
@@ -4499,23 +4686,23 @@
       <c r="D28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="36"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="28"/>
       <c r="N28" s="4"/>
       <c r="O28" s="1"/>
       <c r="T28" s="8" t="s">
         <v>36</v>
       </c>
       <c r="U28" s="1"/>
-      <c r="W28" s="34"/>
-      <c r="Z28" s="34"/>
+      <c r="W28" s="26"/>
+      <c r="Z28" s="26"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="1"/>
-      <c r="AH28" s="34"/>
-      <c r="AJ28" s="36"/>
+      <c r="AH28" s="26"/>
+      <c r="AJ28" s="28"/>
       <c r="AP28" s="4"/>
       <c r="AQ28" s="1"/>
       <c r="AU28" s="1"/>
@@ -4528,23 +4715,23 @@
       <c r="D29" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="36"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="28"/>
       <c r="N29" s="4"/>
       <c r="O29" s="1"/>
       <c r="T29" s="8" t="s">
         <v>257</v>
       </c>
       <c r="U29" s="1"/>
-      <c r="W29" s="34"/>
-      <c r="Z29" s="34"/>
+      <c r="W29" s="26"/>
+      <c r="Z29" s="26"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="1"/>
-      <c r="AH29" s="34"/>
-      <c r="AJ29" s="36"/>
+      <c r="AH29" s="26"/>
+      <c r="AJ29" s="28"/>
       <c r="AP29" s="4"/>
       <c r="AQ29" s="1"/>
       <c r="AU29" s="1"/>
@@ -4557,11 +4744,11 @@
       <c r="D30" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="36"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="28"/>
       <c r="N30" s="4"/>
       <c r="O30" s="1"/>
       <c r="T30" s="8" t="s">
@@ -4582,29 +4769,29 @@
       <c r="D31" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="36"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="28"/>
       <c r="N31" s="4"/>
       <c r="O31" s="1"/>
       <c r="T31" s="8" t="s">
         <v>259</v>
       </c>
       <c r="U31" s="1"/>
-      <c r="W31" s="35" t="s">
+      <c r="W31" s="33" t="s">
         <v>282</v>
       </c>
-      <c r="Z31" s="35" t="s">
+      <c r="Z31" s="33" t="s">
         <v>282</v>
       </c>
       <c r="AA31" s="2"/>
       <c r="AB31" s="1"/>
-      <c r="AH31" s="35" t="s">
+      <c r="AH31" s="33" t="s">
         <v>282</v>
       </c>
-      <c r="AJ31" s="35" t="s">
+      <c r="AJ31" s="33" t="s">
         <v>282</v>
       </c>
       <c r="AP31" s="4"/>
@@ -4619,23 +4806,23 @@
       <c r="D32" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="36"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="28"/>
       <c r="N32" s="4"/>
       <c r="O32" s="1"/>
       <c r="T32" s="8" t="s">
         <v>260</v>
       </c>
       <c r="U32" s="1"/>
-      <c r="W32" s="35"/>
-      <c r="Z32" s="35"/>
+      <c r="W32" s="33"/>
+      <c r="Z32" s="33"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="1"/>
-      <c r="AH32" s="35"/>
-      <c r="AJ32" s="35"/>
+      <c r="AH32" s="33"/>
+      <c r="AJ32" s="33"/>
       <c r="AP32" s="4"/>
       <c r="AQ32" s="1"/>
       <c r="AU32" s="1"/>
@@ -4648,23 +4835,23 @@
       <c r="D33" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="36"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="28"/>
       <c r="N33" s="4"/>
       <c r="O33" s="1"/>
       <c r="T33" s="8" t="s">
         <v>261</v>
       </c>
       <c r="U33" s="1"/>
-      <c r="W33" s="35"/>
-      <c r="Z33" s="35"/>
+      <c r="W33" s="33"/>
+      <c r="Z33" s="33"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="1"/>
-      <c r="AH33" s="35"/>
-      <c r="AJ33" s="35"/>
+      <c r="AH33" s="33"/>
+      <c r="AJ33" s="33"/>
       <c r="AP33" s="4"/>
       <c r="AQ33" s="1"/>
       <c r="AU33" s="1"/>
@@ -4677,19 +4864,19 @@
       <c r="D34" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="K34" s="36"/>
+      <c r="K34" s="28"/>
       <c r="N34" s="4"/>
       <c r="O34" s="1"/>
       <c r="T34" s="8" t="s">
         <v>262</v>
       </c>
       <c r="U34" s="1"/>
-      <c r="W34" s="35"/>
-      <c r="Z34" s="35"/>
+      <c r="W34" s="33"/>
+      <c r="Z34" s="33"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="1"/>
-      <c r="AH34" s="35"/>
-      <c r="AJ34" s="35"/>
+      <c r="AH34" s="33"/>
+      <c r="AJ34" s="33"/>
       <c r="AP34" s="4"/>
       <c r="AQ34" s="1"/>
       <c r="AU34" s="1"/>
@@ -4702,19 +4889,19 @@
       <c r="D35" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="K35" s="36"/>
+      <c r="K35" s="28"/>
       <c r="N35" s="4"/>
       <c r="O35" s="1"/>
       <c r="T35" s="8" t="s">
         <v>263</v>
       </c>
       <c r="U35" s="1"/>
-      <c r="W35" s="35"/>
-      <c r="Z35" s="35"/>
+      <c r="W35" s="33"/>
+      <c r="Z35" s="33"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="1"/>
-      <c r="AH35" s="35"/>
-      <c r="AJ35" s="35"/>
+      <c r="AH35" s="33"/>
+      <c r="AJ35" s="33"/>
       <c r="AP35" s="4"/>
       <c r="AQ35" s="1"/>
       <c r="AU35" s="1"/>
@@ -4724,17 +4911,17 @@
       <c r="D36" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="K36" s="36"/>
+      <c r="K36" s="28"/>
       <c r="N36" s="4"/>
       <c r="O36" s="1"/>
       <c r="T36" s="4"/>
       <c r="U36" s="1"/>
-      <c r="W36" s="35"/>
-      <c r="Z36" s="35"/>
+      <c r="W36" s="33"/>
+      <c r="Z36" s="33"/>
       <c r="AA36" s="2"/>
       <c r="AB36" s="1"/>
-      <c r="AH36" s="35"/>
-      <c r="AJ36" s="35"/>
+      <c r="AH36" s="33"/>
+      <c r="AJ36" s="33"/>
       <c r="AP36" s="4"/>
       <c r="AQ36" s="1"/>
       <c r="AU36" s="1"/>
@@ -4748,12 +4935,12 @@
       <c r="O37" s="1"/>
       <c r="T37" s="4"/>
       <c r="U37" s="1"/>
-      <c r="W37" s="35"/>
-      <c r="Z37" s="35"/>
+      <c r="W37" s="33"/>
+      <c r="Z37" s="33"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="1"/>
-      <c r="AH37" s="35"/>
-      <c r="AJ37" s="35"/>
+      <c r="AH37" s="33"/>
+      <c r="AJ37" s="33"/>
       <c r="AP37" s="4"/>
       <c r="AQ37" s="1"/>
       <c r="AU37" s="1"/>
@@ -4767,12 +4954,12 @@
       <c r="O38" s="1"/>
       <c r="T38" s="4"/>
       <c r="U38" s="1"/>
-      <c r="W38" s="35"/>
-      <c r="Z38" s="35"/>
+      <c r="W38" s="33"/>
+      <c r="Z38" s="33"/>
       <c r="AA38" s="2"/>
       <c r="AB38" s="1"/>
-      <c r="AH38" s="35"/>
-      <c r="AJ38" s="35"/>
+      <c r="AH38" s="33"/>
+      <c r="AJ38" s="33"/>
       <c r="AP38" s="4"/>
       <c r="AQ38" s="1"/>
       <c r="AU38" s="1"/>
@@ -4786,12 +4973,12 @@
       <c r="O39" s="1"/>
       <c r="T39" s="4"/>
       <c r="U39" s="1"/>
-      <c r="W39" s="35"/>
-      <c r="Z39" s="35"/>
+      <c r="W39" s="33"/>
+      <c r="Z39" s="33"/>
       <c r="AA39" s="2"/>
       <c r="AB39" s="1"/>
-      <c r="AH39" s="35"/>
-      <c r="AJ39" s="35"/>
+      <c r="AH39" s="33"/>
+      <c r="AJ39" s="33"/>
       <c r="AP39" s="4"/>
       <c r="AQ39" s="1"/>
       <c r="AU39" s="1"/>
@@ -4805,12 +4992,12 @@
       <c r="O40" s="1"/>
       <c r="T40" s="4"/>
       <c r="U40" s="1"/>
-      <c r="W40" s="35"/>
-      <c r="Z40" s="35"/>
+      <c r="W40" s="33"/>
+      <c r="Z40" s="33"/>
       <c r="AA40" s="2"/>
       <c r="AB40" s="1"/>
-      <c r="AH40" s="35"/>
-      <c r="AJ40" s="35"/>
+      <c r="AH40" s="33"/>
+      <c r="AJ40" s="33"/>
       <c r="AP40" s="4"/>
       <c r="AQ40" s="1"/>
       <c r="AU40" s="1"/>
@@ -6054,6 +6241,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="AN17:AP19"/>
+    <mergeCell ref="AQ17:AQ19"/>
+    <mergeCell ref="AR17:AR19"/>
+    <mergeCell ref="AS17:AS19"/>
+    <mergeCell ref="AT17:AT19"/>
+    <mergeCell ref="AT20:AT26"/>
+    <mergeCell ref="AR20:AR26"/>
+    <mergeCell ref="AS20:AS26"/>
+    <mergeCell ref="AP20:AP26"/>
+    <mergeCell ref="AU20:AU26"/>
+    <mergeCell ref="AQ20:AQ26"/>
+    <mergeCell ref="I20:I33"/>
+    <mergeCell ref="J20:J33"/>
+    <mergeCell ref="N20:N26"/>
+    <mergeCell ref="O20:O26"/>
+    <mergeCell ref="Z31:Z40"/>
+    <mergeCell ref="K27:K36"/>
+    <mergeCell ref="AA20:AA26"/>
+    <mergeCell ref="K20:K26"/>
+    <mergeCell ref="AJ31:AJ40"/>
+    <mergeCell ref="W20:W29"/>
+    <mergeCell ref="W31:W40"/>
+    <mergeCell ref="AH31:AH40"/>
+    <mergeCell ref="Z20:Z29"/>
+    <mergeCell ref="AH20:AH29"/>
+    <mergeCell ref="S20:S26"/>
+    <mergeCell ref="Q20:Q26"/>
+    <mergeCell ref="T20:T26"/>
+    <mergeCell ref="G20:G33"/>
+    <mergeCell ref="H20:H33"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="M20:M26"/>
+    <mergeCell ref="L20:L26"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="D20:D26"/>
+    <mergeCell ref="E20:E26"/>
+    <mergeCell ref="F20:F26"/>
+    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="B17:AM19"/>
+    <mergeCell ref="AG20:AG26"/>
+    <mergeCell ref="P20:P26"/>
+    <mergeCell ref="R20:R26"/>
     <mergeCell ref="AN20:AN26"/>
     <mergeCell ref="AO20:AO26"/>
     <mergeCell ref="U20:U26"/>
@@ -6070,50 +6301,6 @@
     <mergeCell ref="AF20:AF26"/>
     <mergeCell ref="AI20:AI26"/>
     <mergeCell ref="AJ20:AJ29"/>
-    <mergeCell ref="G20:G33"/>
-    <mergeCell ref="H20:H33"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="M20:M26"/>
-    <mergeCell ref="L20:L26"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="D20:D26"/>
-    <mergeCell ref="E20:E26"/>
-    <mergeCell ref="F20:F26"/>
-    <mergeCell ref="C20:C26"/>
-    <mergeCell ref="B17:AM19"/>
-    <mergeCell ref="AG20:AG26"/>
-    <mergeCell ref="P20:P26"/>
-    <mergeCell ref="R20:R26"/>
-    <mergeCell ref="AA20:AA26"/>
-    <mergeCell ref="K20:K26"/>
-    <mergeCell ref="AJ31:AJ40"/>
-    <mergeCell ref="W20:W29"/>
-    <mergeCell ref="W31:W40"/>
-    <mergeCell ref="AH31:AH40"/>
-    <mergeCell ref="Z20:Z29"/>
-    <mergeCell ref="AH20:AH29"/>
-    <mergeCell ref="S20:S26"/>
-    <mergeCell ref="Q20:Q26"/>
-    <mergeCell ref="T20:T26"/>
-    <mergeCell ref="I20:I33"/>
-    <mergeCell ref="J20:J33"/>
-    <mergeCell ref="N20:N26"/>
-    <mergeCell ref="O20:O26"/>
-    <mergeCell ref="Z31:Z40"/>
-    <mergeCell ref="K27:K36"/>
-    <mergeCell ref="AT20:AT26"/>
-    <mergeCell ref="AR20:AR26"/>
-    <mergeCell ref="AS20:AS26"/>
-    <mergeCell ref="AP20:AP26"/>
-    <mergeCell ref="AU20:AU26"/>
-    <mergeCell ref="AQ20:AQ26"/>
-    <mergeCell ref="AN17:AP19"/>
-    <mergeCell ref="AQ17:AQ19"/>
-    <mergeCell ref="AR17:AR19"/>
-    <mergeCell ref="AS17:AS19"/>
-    <mergeCell ref="AT17:AT19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6127,9 +6314,7 @@
   </sheetPr>
   <dimension ref="A1:BB137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -6195,20 +6380,20 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:54" ht="21">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="5" t="s">
         <v>305</v>
       </c>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:54" ht="21">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="5" t="s">
         <v>503</v>
       </c>
@@ -7778,7 +7963,7 @@
       <c r="AI14" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="AJ14" s="43" t="s">
+      <c r="AJ14" s="24" t="s">
         <v>11</v>
       </c>
       <c r="AK14" s="4" t="s">
@@ -8102,7 +8287,7 @@
       <c r="AI16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AJ16" s="43" t="s">
+      <c r="AJ16" s="24" t="s">
         <v>11</v>
       </c>
       <c r="AK16" s="4" t="s">
@@ -9665,672 +9850,672 @@
       <c r="BB28" s="3"/>
     </row>
     <row r="29" spans="1:54" ht="11.25" customHeight="1">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="24"/>
-      <c r="U29" s="24"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="24"/>
-      <c r="Y29" s="24"/>
-      <c r="Z29" s="24"/>
-      <c r="AA29" s="24"/>
-      <c r="AB29" s="24"/>
-      <c r="AC29" s="24"/>
-      <c r="AD29" s="24"/>
-      <c r="AE29" s="24"/>
-      <c r="AF29" s="24"/>
-      <c r="AG29" s="24"/>
-      <c r="AH29" s="24"/>
-      <c r="AI29" s="24"/>
-      <c r="AJ29" s="24"/>
-      <c r="AK29" s="24"/>
-      <c r="AL29" s="24"/>
-      <c r="AM29" s="24"/>
-      <c r="AN29" s="24"/>
-      <c r="AO29" s="24"/>
-      <c r="AP29" s="24"/>
-      <c r="AQ29" s="24"/>
-      <c r="AR29" s="24"/>
-      <c r="AS29" s="24"/>
-      <c r="AT29" s="24"/>
-      <c r="AU29" s="24"/>
-      <c r="AV29" s="24"/>
-      <c r="AW29" s="24"/>
-      <c r="AX29" s="24"/>
-      <c r="AY29" s="25" t="s">
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+      <c r="W29" s="32"/>
+      <c r="X29" s="32"/>
+      <c r="Y29" s="32"/>
+      <c r="Z29" s="32"/>
+      <c r="AA29" s="32"/>
+      <c r="AB29" s="32"/>
+      <c r="AC29" s="32"/>
+      <c r="AD29" s="32"/>
+      <c r="AE29" s="32"/>
+      <c r="AF29" s="32"/>
+      <c r="AG29" s="32"/>
+      <c r="AH29" s="32"/>
+      <c r="AI29" s="32"/>
+      <c r="AJ29" s="32"/>
+      <c r="AK29" s="32"/>
+      <c r="AL29" s="32"/>
+      <c r="AM29" s="32"/>
+      <c r="AN29" s="32"/>
+      <c r="AO29" s="32"/>
+      <c r="AP29" s="32"/>
+      <c r="AQ29" s="32"/>
+      <c r="AR29" s="32"/>
+      <c r="AS29" s="32"/>
+      <c r="AT29" s="32"/>
+      <c r="AU29" s="32"/>
+      <c r="AV29" s="32"/>
+      <c r="AW29" s="32"/>
+      <c r="AX29" s="32"/>
+      <c r="AY29" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="AZ29" s="25" t="s">
+      <c r="AZ29" s="40" t="s">
         <v>295</v>
       </c>
       <c r="BA29" s="3"/>
       <c r="BB29" s="3"/>
     </row>
     <row r="30" spans="1:54" ht="11.25" customHeight="1">
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
-      <c r="Z30" s="24"/>
-      <c r="AA30" s="24"/>
-      <c r="AB30" s="24"/>
-      <c r="AC30" s="24"/>
-      <c r="AD30" s="24"/>
-      <c r="AE30" s="24"/>
-      <c r="AF30" s="24"/>
-      <c r="AG30" s="24"/>
-      <c r="AH30" s="24"/>
-      <c r="AI30" s="24"/>
-      <c r="AJ30" s="24"/>
-      <c r="AK30" s="24"/>
-      <c r="AL30" s="24"/>
-      <c r="AM30" s="24"/>
-      <c r="AN30" s="24"/>
-      <c r="AO30" s="24"/>
-      <c r="AP30" s="24"/>
-      <c r="AQ30" s="24"/>
-      <c r="AR30" s="24"/>
-      <c r="AS30" s="24"/>
-      <c r="AT30" s="24"/>
-      <c r="AU30" s="24"/>
-      <c r="AV30" s="24"/>
-      <c r="AW30" s="24"/>
-      <c r="AX30" s="24"/>
-      <c r="AY30" s="25"/>
-      <c r="AZ30" s="25"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="32"/>
+      <c r="V30" s="32"/>
+      <c r="W30" s="32"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="32"/>
+      <c r="AA30" s="32"/>
+      <c r="AB30" s="32"/>
+      <c r="AC30" s="32"/>
+      <c r="AD30" s="32"/>
+      <c r="AE30" s="32"/>
+      <c r="AF30" s="32"/>
+      <c r="AG30" s="32"/>
+      <c r="AH30" s="32"/>
+      <c r="AI30" s="32"/>
+      <c r="AJ30" s="32"/>
+      <c r="AK30" s="32"/>
+      <c r="AL30" s="32"/>
+      <c r="AM30" s="32"/>
+      <c r="AN30" s="32"/>
+      <c r="AO30" s="32"/>
+      <c r="AP30" s="32"/>
+      <c r="AQ30" s="32"/>
+      <c r="AR30" s="32"/>
+      <c r="AS30" s="32"/>
+      <c r="AT30" s="32"/>
+      <c r="AU30" s="32"/>
+      <c r="AV30" s="32"/>
+      <c r="AW30" s="32"/>
+      <c r="AX30" s="32"/>
+      <c r="AY30" s="40"/>
+      <c r="AZ30" s="40"/>
       <c r="BA30" s="3"/>
       <c r="BB30" s="3"/>
     </row>
     <row r="31" spans="1:54" ht="11.25" customHeight="1">
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
-      <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AB31" s="24"/>
-      <c r="AC31" s="24"/>
-      <c r="AD31" s="24"/>
-      <c r="AE31" s="24"/>
-      <c r="AF31" s="24"/>
-      <c r="AG31" s="24"/>
-      <c r="AH31" s="24"/>
-      <c r="AI31" s="24"/>
-      <c r="AJ31" s="24"/>
-      <c r="AK31" s="24"/>
-      <c r="AL31" s="24"/>
-      <c r="AM31" s="24"/>
-      <c r="AN31" s="24"/>
-      <c r="AO31" s="24"/>
-      <c r="AP31" s="24"/>
-      <c r="AQ31" s="24"/>
-      <c r="AR31" s="24"/>
-      <c r="AS31" s="24"/>
-      <c r="AT31" s="24"/>
-      <c r="AU31" s="24"/>
-      <c r="AV31" s="24"/>
-      <c r="AW31" s="24"/>
-      <c r="AX31" s="24"/>
-      <c r="AY31" s="25"/>
-      <c r="AZ31" s="25"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
+      <c r="Q31" s="32"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="32"/>
+      <c r="T31" s="32"/>
+      <c r="U31" s="32"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="32"/>
+      <c r="AA31" s="32"/>
+      <c r="AB31" s="32"/>
+      <c r="AC31" s="32"/>
+      <c r="AD31" s="32"/>
+      <c r="AE31" s="32"/>
+      <c r="AF31" s="32"/>
+      <c r="AG31" s="32"/>
+      <c r="AH31" s="32"/>
+      <c r="AI31" s="32"/>
+      <c r="AJ31" s="32"/>
+      <c r="AK31" s="32"/>
+      <c r="AL31" s="32"/>
+      <c r="AM31" s="32"/>
+      <c r="AN31" s="32"/>
+      <c r="AO31" s="32"/>
+      <c r="AP31" s="32"/>
+      <c r="AQ31" s="32"/>
+      <c r="AR31" s="32"/>
+      <c r="AS31" s="32"/>
+      <c r="AT31" s="32"/>
+      <c r="AU31" s="32"/>
+      <c r="AV31" s="32"/>
+      <c r="AW31" s="32"/>
+      <c r="AX31" s="32"/>
+      <c r="AY31" s="40"/>
+      <c r="AZ31" s="40"/>
       <c r="BA31" s="3"/>
       <c r="BB31" s="3"/>
     </row>
     <row r="32" spans="1:54" ht="11.25" customHeight="1">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="26" t="s">
         <v>405</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="26" t="s">
         <v>406</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="26" t="s">
         <v>483</v>
       </c>
-      <c r="F32" s="34" t="s">
+      <c r="F32" s="26" t="s">
         <v>467</v>
       </c>
-      <c r="G32" s="34" t="s">
+      <c r="G32" s="26" t="s">
         <v>482</v>
       </c>
-      <c r="H32" s="34" t="s">
+      <c r="H32" s="26" t="s">
         <v>484</v>
       </c>
-      <c r="I32" s="34" t="s">
+      <c r="I32" s="26" t="s">
         <v>408</v>
       </c>
-      <c r="J32" s="34" t="s">
+      <c r="J32" s="26" t="s">
         <v>407</v>
       </c>
-      <c r="K32" s="34" t="s">
+      <c r="K32" s="26" t="s">
         <v>411</v>
       </c>
-      <c r="L32" s="36" t="s">
+      <c r="L32" s="28" t="s">
         <v>469</v>
       </c>
-      <c r="M32" s="36" t="s">
+      <c r="M32" s="28" t="s">
         <v>470</v>
       </c>
-      <c r="N32" s="34" t="s">
+      <c r="N32" s="26" t="s">
         <v>412</v>
       </c>
-      <c r="O32" s="34" t="s">
+      <c r="O32" s="26" t="s">
         <v>413</v>
       </c>
-      <c r="P32" s="34" t="s">
+      <c r="P32" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="Q32" s="34" t="s">
+      <c r="Q32" s="26" t="s">
         <v>432</v>
       </c>
-      <c r="R32" s="34" t="s">
+      <c r="R32" s="26" t="s">
         <v>409</v>
       </c>
-      <c r="S32" s="34" t="s">
+      <c r="S32" s="26" t="s">
         <v>410</v>
       </c>
-      <c r="T32" s="34" t="s">
+      <c r="T32" s="26" t="s">
         <v>416</v>
       </c>
-      <c r="U32" s="34" t="s">
+      <c r="U32" s="26" t="s">
         <v>415</v>
       </c>
-      <c r="V32" s="36" t="s">
+      <c r="V32" s="28" t="s">
         <v>450</v>
       </c>
-      <c r="W32" s="36" t="s">
+      <c r="W32" s="28" t="s">
         <v>451</v>
       </c>
-      <c r="X32" s="36" t="s">
+      <c r="X32" s="28" t="s">
         <v>452</v>
       </c>
-      <c r="Y32" s="36" t="s">
+      <c r="Y32" s="28" t="s">
         <v>419</v>
       </c>
-      <c r="Z32" s="34" t="s">
+      <c r="Z32" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="AA32" s="34" t="s">
+      <c r="AA32" s="26" t="s">
         <v>418</v>
       </c>
-      <c r="AB32" s="36" t="s">
+      <c r="AB32" s="28" t="s">
         <v>420</v>
       </c>
-      <c r="AC32" s="36" t="s">
+      <c r="AC32" s="28" t="s">
         <v>453</v>
       </c>
-      <c r="AD32" s="36" t="s">
+      <c r="AD32" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="AE32" s="36" t="s">
+      <c r="AE32" s="28" t="s">
         <v>455</v>
       </c>
-      <c r="AF32" s="36" t="s">
+      <c r="AF32" s="28" t="s">
         <v>462</v>
       </c>
-      <c r="AG32" s="36" t="s">
+      <c r="AG32" s="28" t="s">
         <v>421</v>
       </c>
-      <c r="AH32" s="36" t="s">
+      <c r="AH32" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="AI32" s="36" t="s">
+      <c r="AI32" s="28" t="s">
         <v>457</v>
       </c>
-      <c r="AJ32" s="36" t="s">
+      <c r="AJ32" s="28" t="s">
         <v>458</v>
       </c>
-      <c r="AK32" s="36" t="s">
+      <c r="AK32" s="28" t="s">
         <v>464</v>
       </c>
-      <c r="AL32" s="36" t="s">
+      <c r="AL32" s="28" t="s">
         <v>422</v>
       </c>
-      <c r="AM32" s="36" t="s">
+      <c r="AM32" s="28" t="s">
         <v>433</v>
       </c>
-      <c r="AN32" s="36" t="s">
+      <c r="AN32" s="28" t="s">
         <v>459</v>
       </c>
-      <c r="AO32" s="36" t="s">
+      <c r="AO32" s="28" t="s">
         <v>460</v>
       </c>
-      <c r="AP32" s="36" t="s">
+      <c r="AP32" s="28" t="s">
         <v>461</v>
       </c>
-      <c r="AQ32" s="36" t="s">
+      <c r="AQ32" s="28" t="s">
         <v>424</v>
       </c>
-      <c r="AR32" s="36" t="s">
+      <c r="AR32" s="28" t="s">
         <v>423</v>
       </c>
-      <c r="AS32" s="36" t="s">
+      <c r="AS32" s="28" t="s">
         <v>465</v>
       </c>
-      <c r="AT32" s="36" t="s">
+      <c r="AT32" s="28" t="s">
         <v>466</v>
       </c>
-      <c r="AU32" s="36" t="s">
+      <c r="AU32" s="28" t="s">
         <v>434</v>
       </c>
-      <c r="AV32" s="36" t="s">
+      <c r="AV32" s="28" t="s">
         <v>435</v>
       </c>
-      <c r="AW32" s="36" t="s">
+      <c r="AW32" s="28" t="s">
         <v>486</v>
       </c>
-      <c r="AX32" s="36" t="s">
+      <c r="AX32" s="28" t="s">
         <v>487</v>
       </c>
-      <c r="AY32" s="27" t="s">
+      <c r="AY32" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="AZ32" s="28" t="s">
+      <c r="AZ32" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="BA32" s="30" t="s">
+      <c r="BA32" s="38" t="s">
         <v>468</v>
       </c>
       <c r="BB32" s="3"/>
     </row>
     <row r="33" spans="1:54" ht="11.25" customHeight="1">
-      <c r="A33" s="41"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="34"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="34"/>
-      <c r="T33" s="34"/>
-      <c r="U33" s="34"/>
-      <c r="V33" s="36"/>
-      <c r="W33" s="36"/>
-      <c r="X33" s="36"/>
-      <c r="Y33" s="36"/>
-      <c r="Z33" s="34"/>
-      <c r="AA33" s="34"/>
-      <c r="AB33" s="36"/>
-      <c r="AC33" s="36"/>
-      <c r="AD33" s="36"/>
-      <c r="AE33" s="36"/>
-      <c r="AF33" s="36"/>
-      <c r="AG33" s="36"/>
-      <c r="AH33" s="36"/>
-      <c r="AI33" s="36"/>
-      <c r="AJ33" s="36"/>
-      <c r="AK33" s="36"/>
-      <c r="AL33" s="36"/>
-      <c r="AM33" s="36"/>
-      <c r="AN33" s="36"/>
-      <c r="AO33" s="36"/>
-      <c r="AP33" s="36"/>
-      <c r="AQ33" s="36"/>
-      <c r="AR33" s="36"/>
-      <c r="AS33" s="36"/>
-      <c r="AT33" s="36"/>
-      <c r="AU33" s="36"/>
-      <c r="AV33" s="36"/>
-      <c r="AW33" s="36"/>
-      <c r="AX33" s="36"/>
-      <c r="AY33" s="27"/>
-      <c r="AZ33" s="28"/>
-      <c r="BA33" s="30"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="V33" s="28"/>
+      <c r="W33" s="28"/>
+      <c r="X33" s="28"/>
+      <c r="Y33" s="28"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="28"/>
+      <c r="AC33" s="28"/>
+      <c r="AD33" s="28"/>
+      <c r="AE33" s="28"/>
+      <c r="AF33" s="28"/>
+      <c r="AG33" s="28"/>
+      <c r="AH33" s="28"/>
+      <c r="AI33" s="28"/>
+      <c r="AJ33" s="28"/>
+      <c r="AK33" s="28"/>
+      <c r="AL33" s="28"/>
+      <c r="AM33" s="28"/>
+      <c r="AN33" s="28"/>
+      <c r="AO33" s="28"/>
+      <c r="AP33" s="28"/>
+      <c r="AQ33" s="28"/>
+      <c r="AR33" s="28"/>
+      <c r="AS33" s="28"/>
+      <c r="AT33" s="28"/>
+      <c r="AU33" s="28"/>
+      <c r="AV33" s="28"/>
+      <c r="AW33" s="28"/>
+      <c r="AX33" s="28"/>
+      <c r="AY33" s="36"/>
+      <c r="AZ33" s="37"/>
+      <c r="BA33" s="38"/>
       <c r="BB33" s="3"/>
     </row>
     <row r="34" spans="1:54" ht="11.25" customHeight="1">
-      <c r="A34" s="41"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="34"/>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="34"/>
-      <c r="T34" s="34"/>
-      <c r="U34" s="34"/>
-      <c r="V34" s="36"/>
-      <c r="W34" s="36"/>
-      <c r="X34" s="36"/>
-      <c r="Y34" s="36"/>
-      <c r="Z34" s="34"/>
-      <c r="AA34" s="34"/>
-      <c r="AB34" s="36"/>
-      <c r="AC34" s="36"/>
-      <c r="AD34" s="36"/>
-      <c r="AE34" s="36"/>
-      <c r="AF34" s="36"/>
-      <c r="AG34" s="36"/>
-      <c r="AH34" s="36"/>
-      <c r="AI34" s="36"/>
-      <c r="AJ34" s="36"/>
-      <c r="AK34" s="36"/>
-      <c r="AL34" s="36"/>
-      <c r="AM34" s="36"/>
-      <c r="AN34" s="36"/>
-      <c r="AO34" s="36"/>
-      <c r="AP34" s="36"/>
-      <c r="AQ34" s="36"/>
-      <c r="AR34" s="36"/>
-      <c r="AS34" s="36"/>
-      <c r="AT34" s="36"/>
-      <c r="AU34" s="36"/>
-      <c r="AV34" s="36"/>
-      <c r="AW34" s="36"/>
-      <c r="AX34" s="36"/>
-      <c r="AY34" s="27"/>
-      <c r="AZ34" s="28"/>
-      <c r="BA34" s="30"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="26"/>
+      <c r="U34" s="26"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="28"/>
+      <c r="X34" s="28"/>
+      <c r="Y34" s="28"/>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="28"/>
+      <c r="AC34" s="28"/>
+      <c r="AD34" s="28"/>
+      <c r="AE34" s="28"/>
+      <c r="AF34" s="28"/>
+      <c r="AG34" s="28"/>
+      <c r="AH34" s="28"/>
+      <c r="AI34" s="28"/>
+      <c r="AJ34" s="28"/>
+      <c r="AK34" s="28"/>
+      <c r="AL34" s="28"/>
+      <c r="AM34" s="28"/>
+      <c r="AN34" s="28"/>
+      <c r="AO34" s="28"/>
+      <c r="AP34" s="28"/>
+      <c r="AQ34" s="28"/>
+      <c r="AR34" s="28"/>
+      <c r="AS34" s="28"/>
+      <c r="AT34" s="28"/>
+      <c r="AU34" s="28"/>
+      <c r="AV34" s="28"/>
+      <c r="AW34" s="28"/>
+      <c r="AX34" s="28"/>
+      <c r="AY34" s="36"/>
+      <c r="AZ34" s="37"/>
+      <c r="BA34" s="38"/>
       <c r="BB34" s="3"/>
     </row>
     <row r="35" spans="1:54" ht="11.25" customHeight="1">
-      <c r="A35" s="41"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="34"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="34"/>
-      <c r="T35" s="34"/>
-      <c r="U35" s="34"/>
-      <c r="V35" s="36"/>
-      <c r="W35" s="36"/>
-      <c r="X35" s="36"/>
-      <c r="Y35" s="36"/>
-      <c r="Z35" s="34"/>
-      <c r="AA35" s="34"/>
-      <c r="AB35" s="36"/>
-      <c r="AC35" s="36"/>
-      <c r="AD35" s="36"/>
-      <c r="AE35" s="36"/>
-      <c r="AF35" s="36"/>
-      <c r="AG35" s="36"/>
-      <c r="AH35" s="36"/>
-      <c r="AI35" s="36"/>
-      <c r="AJ35" s="36"/>
-      <c r="AK35" s="36"/>
-      <c r="AL35" s="36"/>
-      <c r="AM35" s="36"/>
-      <c r="AN35" s="36"/>
-      <c r="AO35" s="36"/>
-      <c r="AP35" s="36"/>
-      <c r="AQ35" s="36"/>
-      <c r="AR35" s="36"/>
-      <c r="AS35" s="36"/>
-      <c r="AT35" s="36"/>
-      <c r="AU35" s="36"/>
-      <c r="AV35" s="36"/>
-      <c r="AW35" s="36"/>
-      <c r="AX35" s="36"/>
-      <c r="AY35" s="27"/>
-      <c r="AZ35" s="28"/>
-      <c r="BA35" s="30"/>
+      <c r="A35" s="42"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
+      <c r="P35" s="26"/>
+      <c r="Q35" s="26"/>
+      <c r="R35" s="26"/>
+      <c r="S35" s="26"/>
+      <c r="T35" s="26"/>
+      <c r="U35" s="26"/>
+      <c r="V35" s="28"/>
+      <c r="W35" s="28"/>
+      <c r="X35" s="28"/>
+      <c r="Y35" s="28"/>
+      <c r="Z35" s="26"/>
+      <c r="AA35" s="26"/>
+      <c r="AB35" s="28"/>
+      <c r="AC35" s="28"/>
+      <c r="AD35" s="28"/>
+      <c r="AE35" s="28"/>
+      <c r="AF35" s="28"/>
+      <c r="AG35" s="28"/>
+      <c r="AH35" s="28"/>
+      <c r="AI35" s="28"/>
+      <c r="AJ35" s="28"/>
+      <c r="AK35" s="28"/>
+      <c r="AL35" s="28"/>
+      <c r="AM35" s="28"/>
+      <c r="AN35" s="28"/>
+      <c r="AO35" s="28"/>
+      <c r="AP35" s="28"/>
+      <c r="AQ35" s="28"/>
+      <c r="AR35" s="28"/>
+      <c r="AS35" s="28"/>
+      <c r="AT35" s="28"/>
+      <c r="AU35" s="28"/>
+      <c r="AV35" s="28"/>
+      <c r="AW35" s="28"/>
+      <c r="AX35" s="28"/>
+      <c r="AY35" s="36"/>
+      <c r="AZ35" s="37"/>
+      <c r="BA35" s="38"/>
       <c r="BB35" s="3"/>
     </row>
     <row r="36" spans="1:54">
-      <c r="A36" s="41"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="34"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="34"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="36"/>
-      <c r="W36" s="36"/>
-      <c r="X36" s="36"/>
-      <c r="Y36" s="36"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="34"/>
-      <c r="AB36" s="36"/>
-      <c r="AC36" s="36"/>
-      <c r="AD36" s="36"/>
-      <c r="AE36" s="36"/>
-      <c r="AF36" s="36"/>
-      <c r="AG36" s="36"/>
-      <c r="AH36" s="36"/>
-      <c r="AI36" s="36"/>
-      <c r="AJ36" s="36"/>
-      <c r="AK36" s="36"/>
-      <c r="AL36" s="36"/>
-      <c r="AM36" s="36"/>
-      <c r="AN36" s="36"/>
-      <c r="AO36" s="36"/>
-      <c r="AP36" s="36"/>
-      <c r="AQ36" s="36"/>
-      <c r="AR36" s="36"/>
-      <c r="AS36" s="36"/>
-      <c r="AT36" s="36"/>
-      <c r="AU36" s="36"/>
-      <c r="AV36" s="36"/>
-      <c r="AW36" s="36"/>
-      <c r="AX36" s="36"/>
-      <c r="AY36" s="27"/>
-      <c r="AZ36" s="28"/>
-      <c r="BA36" s="30"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="26"/>
+      <c r="O36" s="26"/>
+      <c r="P36" s="26"/>
+      <c r="Q36" s="26"/>
+      <c r="R36" s="26"/>
+      <c r="S36" s="26"/>
+      <c r="T36" s="26"/>
+      <c r="U36" s="26"/>
+      <c r="V36" s="28"/>
+      <c r="W36" s="28"/>
+      <c r="X36" s="28"/>
+      <c r="Y36" s="28"/>
+      <c r="Z36" s="26"/>
+      <c r="AA36" s="26"/>
+      <c r="AB36" s="28"/>
+      <c r="AC36" s="28"/>
+      <c r="AD36" s="28"/>
+      <c r="AE36" s="28"/>
+      <c r="AF36" s="28"/>
+      <c r="AG36" s="28"/>
+      <c r="AH36" s="28"/>
+      <c r="AI36" s="28"/>
+      <c r="AJ36" s="28"/>
+      <c r="AK36" s="28"/>
+      <c r="AL36" s="28"/>
+      <c r="AM36" s="28"/>
+      <c r="AN36" s="28"/>
+      <c r="AO36" s="28"/>
+      <c r="AP36" s="28"/>
+      <c r="AQ36" s="28"/>
+      <c r="AR36" s="28"/>
+      <c r="AS36" s="28"/>
+      <c r="AT36" s="28"/>
+      <c r="AU36" s="28"/>
+      <c r="AV36" s="28"/>
+      <c r="AW36" s="28"/>
+      <c r="AX36" s="28"/>
+      <c r="AY36" s="36"/>
+      <c r="AZ36" s="37"/>
+      <c r="BA36" s="38"/>
       <c r="BB36" s="3"/>
     </row>
     <row r="37" spans="1:54">
-      <c r="A37" s="41"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="34"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="34"/>
-      <c r="S37" s="34"/>
-      <c r="T37" s="34"/>
-      <c r="U37" s="34"/>
-      <c r="V37" s="36"/>
-      <c r="W37" s="36"/>
-      <c r="X37" s="36"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="34"/>
-      <c r="AA37" s="34"/>
-      <c r="AB37" s="36"/>
-      <c r="AC37" s="36"/>
-      <c r="AD37" s="36"/>
-      <c r="AE37" s="36"/>
-      <c r="AF37" s="36"/>
-      <c r="AG37" s="36"/>
-      <c r="AH37" s="36"/>
-      <c r="AI37" s="36"/>
-      <c r="AJ37" s="36"/>
-      <c r="AK37" s="36"/>
-      <c r="AL37" s="36"/>
-      <c r="AM37" s="36"/>
-      <c r="AN37" s="36"/>
-      <c r="AO37" s="36"/>
-      <c r="AP37" s="36"/>
-      <c r="AQ37" s="36"/>
-      <c r="AR37" s="36"/>
-      <c r="AS37" s="36"/>
-      <c r="AT37" s="36"/>
-      <c r="AU37" s="36"/>
-      <c r="AV37" s="36"/>
-      <c r="AW37" s="36"/>
-      <c r="AX37" s="36"/>
-      <c r="AY37" s="27"/>
-      <c r="AZ37" s="28"/>
-      <c r="BA37" s="30"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="26"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="28"/>
+      <c r="X37" s="28"/>
+      <c r="Y37" s="28"/>
+      <c r="Z37" s="26"/>
+      <c r="AA37" s="26"/>
+      <c r="AB37" s="28"/>
+      <c r="AC37" s="28"/>
+      <c r="AD37" s="28"/>
+      <c r="AE37" s="28"/>
+      <c r="AF37" s="28"/>
+      <c r="AG37" s="28"/>
+      <c r="AH37" s="28"/>
+      <c r="AI37" s="28"/>
+      <c r="AJ37" s="28"/>
+      <c r="AK37" s="28"/>
+      <c r="AL37" s="28"/>
+      <c r="AM37" s="28"/>
+      <c r="AN37" s="28"/>
+      <c r="AO37" s="28"/>
+      <c r="AP37" s="28"/>
+      <c r="AQ37" s="28"/>
+      <c r="AR37" s="28"/>
+      <c r="AS37" s="28"/>
+      <c r="AT37" s="28"/>
+      <c r="AU37" s="28"/>
+      <c r="AV37" s="28"/>
+      <c r="AW37" s="28"/>
+      <c r="AX37" s="28"/>
+      <c r="AY37" s="36"/>
+      <c r="AZ37" s="37"/>
+      <c r="BA37" s="38"/>
       <c r="BB37" s="3"/>
     </row>
     <row r="38" spans="1:54">
-      <c r="A38" s="42"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
-      <c r="S38" s="34"/>
-      <c r="T38" s="34"/>
-      <c r="U38" s="34"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="36"/>
-      <c r="X38" s="36"/>
-      <c r="Y38" s="36"/>
-      <c r="Z38" s="34"/>
-      <c r="AA38" s="34"/>
-      <c r="AB38" s="36"/>
-      <c r="AC38" s="36"/>
-      <c r="AD38" s="36"/>
-      <c r="AE38" s="36"/>
-      <c r="AF38" s="36"/>
-      <c r="AG38" s="36"/>
-      <c r="AH38" s="36"/>
-      <c r="AI38" s="36"/>
-      <c r="AJ38" s="36"/>
-      <c r="AK38" s="36"/>
-      <c r="AL38" s="36"/>
-      <c r="AM38" s="36"/>
-      <c r="AN38" s="36"/>
-      <c r="AO38" s="36"/>
-      <c r="AP38" s="36"/>
-      <c r="AQ38" s="36"/>
-      <c r="AR38" s="36"/>
-      <c r="AS38" s="36"/>
-      <c r="AT38" s="36"/>
-      <c r="AU38" s="36"/>
-      <c r="AV38" s="36"/>
-      <c r="AW38" s="36"/>
-      <c r="AX38" s="36"/>
-      <c r="AY38" s="27"/>
-      <c r="AZ38" s="28"/>
-      <c r="BA38" s="30"/>
+      <c r="A38" s="43"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="26"/>
+      <c r="O38" s="26"/>
+      <c r="P38" s="26"/>
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26"/>
+      <c r="S38" s="26"/>
+      <c r="T38" s="26"/>
+      <c r="U38" s="26"/>
+      <c r="V38" s="28"/>
+      <c r="W38" s="28"/>
+      <c r="X38" s="28"/>
+      <c r="Y38" s="28"/>
+      <c r="Z38" s="26"/>
+      <c r="AA38" s="26"/>
+      <c r="AB38" s="28"/>
+      <c r="AC38" s="28"/>
+      <c r="AD38" s="28"/>
+      <c r="AE38" s="28"/>
+      <c r="AF38" s="28"/>
+      <c r="AG38" s="28"/>
+      <c r="AH38" s="28"/>
+      <c r="AI38" s="28"/>
+      <c r="AJ38" s="28"/>
+      <c r="AK38" s="28"/>
+      <c r="AL38" s="28"/>
+      <c r="AM38" s="28"/>
+      <c r="AN38" s="28"/>
+      <c r="AO38" s="28"/>
+      <c r="AP38" s="28"/>
+      <c r="AQ38" s="28"/>
+      <c r="AR38" s="28"/>
+      <c r="AS38" s="28"/>
+      <c r="AT38" s="28"/>
+      <c r="AU38" s="28"/>
+      <c r="AV38" s="28"/>
+      <c r="AW38" s="28"/>
+      <c r="AX38" s="28"/>
+      <c r="AY38" s="36"/>
+      <c r="AZ38" s="37"/>
+      <c r="BA38" s="38"/>
       <c r="BB38" s="3"/>
     </row>
     <row r="39" spans="1:54">
@@ -11894,6 +12079,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="BA32:BA38"/>
+    <mergeCell ref="AY29:AY31"/>
+    <mergeCell ref="AZ29:AZ31"/>
+    <mergeCell ref="AY32:AY38"/>
+    <mergeCell ref="AZ32:AZ38"/>
+    <mergeCell ref="AS32:AS38"/>
+    <mergeCell ref="AT32:AT38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="AF32:AF38"/>
+    <mergeCell ref="AK32:AK38"/>
+    <mergeCell ref="AI32:AI38"/>
+    <mergeCell ref="AJ32:AJ38"/>
+    <mergeCell ref="AN32:AN38"/>
+    <mergeCell ref="AO32:AO38"/>
+    <mergeCell ref="R32:R38"/>
+    <mergeCell ref="S32:S38"/>
+    <mergeCell ref="K32:K38"/>
+    <mergeCell ref="N32:N38"/>
+    <mergeCell ref="O32:O38"/>
+    <mergeCell ref="P32:P38"/>
+    <mergeCell ref="AV32:AV38"/>
+    <mergeCell ref="AW32:AW38"/>
+    <mergeCell ref="V32:V38"/>
+    <mergeCell ref="W32:W38"/>
+    <mergeCell ref="X32:X38"/>
+    <mergeCell ref="AC32:AC38"/>
+    <mergeCell ref="Z32:Z38"/>
+    <mergeCell ref="AA32:AA38"/>
+    <mergeCell ref="Y32:Y38"/>
+    <mergeCell ref="AB32:AB38"/>
+    <mergeCell ref="AG32:AG38"/>
+    <mergeCell ref="AL32:AL38"/>
+    <mergeCell ref="AD32:AD38"/>
+    <mergeCell ref="AE32:AE38"/>
+    <mergeCell ref="AH32:AH38"/>
+    <mergeCell ref="AU32:AU38"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="D32:D38"/>
+    <mergeCell ref="J32:J38"/>
+    <mergeCell ref="I32:I38"/>
     <mergeCell ref="AX32:AX38"/>
     <mergeCell ref="B29:AX31"/>
     <mergeCell ref="A2:B2"/>
@@ -11910,48 +12137,6 @@
     <mergeCell ref="AM32:AM38"/>
     <mergeCell ref="Q32:Q38"/>
     <mergeCell ref="A32:A38"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="D32:D38"/>
-    <mergeCell ref="J32:J38"/>
-    <mergeCell ref="I32:I38"/>
-    <mergeCell ref="AV32:AV38"/>
-    <mergeCell ref="AW32:AW38"/>
-    <mergeCell ref="V32:V38"/>
-    <mergeCell ref="W32:W38"/>
-    <mergeCell ref="X32:X38"/>
-    <mergeCell ref="AC32:AC38"/>
-    <mergeCell ref="Z32:Z38"/>
-    <mergeCell ref="AA32:AA38"/>
-    <mergeCell ref="Y32:Y38"/>
-    <mergeCell ref="AB32:AB38"/>
-    <mergeCell ref="AG32:AG38"/>
-    <mergeCell ref="AL32:AL38"/>
-    <mergeCell ref="AD32:AD38"/>
-    <mergeCell ref="AE32:AE38"/>
-    <mergeCell ref="AH32:AH38"/>
-    <mergeCell ref="AU32:AU38"/>
-    <mergeCell ref="AS32:AS38"/>
-    <mergeCell ref="AT32:AT38"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="AF32:AF38"/>
-    <mergeCell ref="AK32:AK38"/>
-    <mergeCell ref="AI32:AI38"/>
-    <mergeCell ref="AJ32:AJ38"/>
-    <mergeCell ref="AN32:AN38"/>
-    <mergeCell ref="AO32:AO38"/>
-    <mergeCell ref="R32:R38"/>
-    <mergeCell ref="S32:S38"/>
-    <mergeCell ref="K32:K38"/>
-    <mergeCell ref="N32:N38"/>
-    <mergeCell ref="O32:O38"/>
-    <mergeCell ref="P32:P38"/>
-    <mergeCell ref="BA32:BA38"/>
-    <mergeCell ref="AY29:AY31"/>
-    <mergeCell ref="AZ29:AZ31"/>
-    <mergeCell ref="AY32:AY38"/>
-    <mergeCell ref="AZ32:AZ38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11963,27 +12148,25 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:BB10"/>
+  <dimension ref="A1:BB36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" style="18" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="35.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="41.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="18" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="34.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="37.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.85546875" style="4" customWidth="1"/>
     <col min="16" max="16" width="18.5703125" style="4" customWidth="1"/>
@@ -12033,25 +12216,28 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:54" ht="21">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="5" t="s">
         <v>504</v>
       </c>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:54" ht="21">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="M3" s="5"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="5" spans="1:54">
-      <c r="H5" s="18"/>
+      <c r="G5" s="18"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="T5" s="18"/>
@@ -12066,8 +12252,46 @@
       <c r="BA5" s="3"/>
       <c r="BB5" s="3"/>
     </row>
-    <row r="6" spans="1:54">
-      <c r="H6" s="18"/>
+    <row r="6" spans="1:54" ht="20.25" customHeight="1">
+      <c r="A6" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>506</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>508</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>511</v>
+      </c>
+      <c r="I6" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="47" t="s">
+        <v>509</v>
+      </c>
+      <c r="K6" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="L6" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="47" t="s">
+        <v>8</v>
+      </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="T6" s="18"/>
@@ -12083,7 +12307,45 @@
       <c r="BB6" s="3"/>
     </row>
     <row r="7" spans="1:54">
-      <c r="H7" s="18"/>
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>513</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="T7" s="18"/>
@@ -12099,7 +12361,45 @@
       <c r="BB7" s="3"/>
     </row>
     <row r="8" spans="1:54">
-      <c r="H8" s="18"/>
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>516</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="T8" s="18"/>
@@ -12115,7 +12415,45 @@
       <c r="BB8" s="3"/>
     </row>
     <row r="9" spans="1:54">
-      <c r="H9" s="18"/>
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>520</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>521</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>522</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="T9" s="18"/>
@@ -12131,25 +12469,570 @@
       <c r="BB9" s="3"/>
     </row>
     <row r="10" spans="1:54">
-      <c r="H10" s="18"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
       <c r="T10" s="18"/>
-      <c r="W10" s="2"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
-      <c r="Z10" s="19"/>
-      <c r="AG10" s="1"/>
-      <c r="AK10" s="1"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="4"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+      <c r="AG10" s="4"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
+      <c r="AJ10" s="4"/>
       <c r="AL10" s="4"/>
+      <c r="AM10" s="4"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="4"/>
+      <c r="AP10" s="4"/>
+      <c r="AQ10" s="4"/>
+      <c r="AR10" s="4"/>
       <c r="AS10" s="4"/>
       <c r="AT10" s="4"/>
+      <c r="AU10" s="4"/>
+      <c r="AV10" s="4"/>
+      <c r="AW10" s="4"/>
+      <c r="AX10" s="4"/>
       <c r="BA10" s="3"/>
       <c r="BB10" s="3"/>
     </row>
+    <row r="11" spans="1:54">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>528</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>529</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>533</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>539</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="B18" s="32" t="s">
+        <v>550</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32" t="s">
+        <v>553</v>
+      </c>
+      <c r="K18" s="32"/>
+      <c r="L18" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="M18" s="40" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>551</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>552</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>554</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>468</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>557</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="L21" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="M21" s="37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="45"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="37"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="45"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="37"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="45"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="37"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="45"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="45"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="37"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="46"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="37"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="E29" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="E30" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="E31" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="E32" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="19">
+    <mergeCell ref="K21:K27"/>
+    <mergeCell ref="B18:I20"/>
+    <mergeCell ref="J18:K20"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="L21:L27"/>
+    <mergeCell ref="M21:M27"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="G21:G27"/>
+    <mergeCell ref="I21:I27"/>
+    <mergeCell ref="J21:J27"/>
+    <mergeCell ref="H21:H27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E21:E27"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="B21:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>